<commit_message>
Removed # of request from scrapper
</commit_message>
<xml_diff>
--- a/analytics_csv/monthly_data.xlsx
+++ b/analytics_csv/monthly_data.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H128"/>
+  <dimension ref="A1:H129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -576,13 +576,13 @@
         <v>106.0899963378906</v>
       </c>
       <c r="F5" t="n">
-        <v>97.51000213623047</v>
+        <v>97.51000213623048</v>
       </c>
       <c r="G5" t="n">
-        <v>8.579994201660156</v>
+        <v>8.579994201660142</v>
       </c>
       <c r="H5" t="n">
-        <v>8.799091389284468</v>
+        <v>8.799091389284452</v>
       </c>
     </row>
     <row r="6">
@@ -842,7 +842,7 @@
         <v>176.0440063476562</v>
       </c>
       <c r="H15" t="n">
-        <v>39.32775467311988</v>
+        <v>39.32775467311986</v>
       </c>
     </row>
     <row r="16">
@@ -911,7 +911,7 @@
         <v>461.4599914550781</v>
       </c>
       <c r="E18" t="n">
-        <v>477.7630004882812</v>
+        <v>477.7630004882813</v>
       </c>
       <c r="F18" t="n">
         <v>586.2020263671875</v>
@@ -920,7 +920,7 @@
         <v>-108.4390258789062</v>
       </c>
       <c r="H18" t="n">
-        <v>-18.49857574715748</v>
+        <v>-18.49857574715747</v>
       </c>
     </row>
     <row r="19">
@@ -1009,7 +1009,7 @@
         <v>341.2678705030872</v>
       </c>
       <c r="C22" t="n">
-        <v>381.3150024414062</v>
+        <v>381.3150024414063</v>
       </c>
       <c r="D22" t="n">
         <v>310.7369995117188</v>
@@ -1044,13 +1044,13 @@
         <v>217.4640045166016</v>
       </c>
       <c r="F23" t="n">
-        <v>320.4349975585938</v>
+        <v>320.4349975585937</v>
       </c>
       <c r="G23" t="n">
-        <v>-102.9709930419922</v>
+        <v>-102.9709930419921</v>
       </c>
       <c r="H23" t="n">
-        <v>-32.13475239175872</v>
+        <v>-32.1347523917587</v>
       </c>
     </row>
     <row r="24">
@@ -1064,7 +1064,7 @@
         <v>257.3210144042969</v>
       </c>
       <c r="D24" t="n">
-        <v>217.1109924316406</v>
+        <v>217.1109924316407</v>
       </c>
       <c r="E24" t="n">
         <v>254.2630004882812</v>
@@ -1125,10 +1125,10 @@
         <v>244.2230072021484</v>
       </c>
       <c r="G26" t="n">
-        <v>-8.0780029296875</v>
+        <v>-8.078002929687528</v>
       </c>
       <c r="H26" t="n">
-        <v>-3.307633880292519</v>
+        <v>-3.30763388029253</v>
       </c>
     </row>
     <row r="27">
@@ -1151,10 +1151,10 @@
         <v>235.9389953613281</v>
       </c>
       <c r="G27" t="n">
-        <v>-5.748992919921875</v>
+        <v>-5.748992919921818</v>
       </c>
       <c r="H27" t="n">
-        <v>-2.436643807488285</v>
+        <v>-2.436643807488262</v>
       </c>
     </row>
     <row r="28">
@@ -1177,10 +1177,10 @@
         <v>230.2330017089844</v>
       </c>
       <c r="G28" t="n">
-        <v>32.8389892578125</v>
+        <v>32.83898925781247</v>
       </c>
       <c r="H28" t="n">
-        <v>14.26337189458232</v>
+        <v>14.2633718945823</v>
       </c>
     </row>
     <row r="29">
@@ -1223,16 +1223,16 @@
         <v>210.4949951171875</v>
       </c>
       <c r="E30" t="n">
-        <v>230.0559997558594</v>
+        <v>230.0559997558593</v>
       </c>
       <c r="F30" t="n">
         <v>284.6860046386719</v>
       </c>
       <c r="G30" t="n">
-        <v>-54.6300048828125</v>
+        <v>-54.63000488281253</v>
       </c>
       <c r="H30" t="n">
-        <v>-19.18956464057648</v>
+        <v>-19.18956464057649</v>
       </c>
     </row>
     <row r="31">
@@ -1249,16 +1249,16 @@
         <v>227.0850067138672</v>
       </c>
       <c r="E31" t="n">
-        <v>236.0599975585938</v>
+        <v>236.0599975585937</v>
       </c>
       <c r="F31" t="n">
         <v>230.2559967041016</v>
       </c>
       <c r="G31" t="n">
-        <v>5.804000854492188</v>
+        <v>5.804000854492131</v>
       </c>
       <c r="H31" t="n">
-        <v>2.520673049810216</v>
+        <v>2.520673049810191</v>
       </c>
     </row>
     <row r="32">
@@ -1281,10 +1281,10 @@
         <v>236.0039978027344</v>
       </c>
       <c r="G32" t="n">
-        <v>78.1619873046875</v>
+        <v>78.16198730468747</v>
       </c>
       <c r="H32" t="n">
-        <v>33.1189251166922</v>
+        <v>33.11892511669218</v>
       </c>
     </row>
     <row r="33">
@@ -1356,13 +1356,13 @@
         <v>368.7669982910156</v>
       </c>
       <c r="F35" t="n">
-        <v>430.7210083007812</v>
+        <v>430.7210083007813</v>
       </c>
       <c r="G35" t="n">
-        <v>-61.95401000976562</v>
+        <v>-61.95401000976568</v>
       </c>
       <c r="H35" t="n">
-        <v>-14.38379108884837</v>
+        <v>-14.38379108884838</v>
       </c>
     </row>
     <row r="36">
@@ -1633,7 +1633,7 @@
         <v>828.0603558940272</v>
       </c>
       <c r="C46" t="n">
-        <v>975.9210205078125</v>
+        <v>975.9210205078124</v>
       </c>
       <c r="D46" t="n">
         <v>756.7739868164062</v>
@@ -3147,16 +3147,16 @@
         <v>47711.48646346977</v>
       </c>
       <c r="E104" t="n">
-        <v>61318.95776660598</v>
+        <v>61318.95776660599</v>
       </c>
       <c r="F104" t="n">
         <v>43816.74064429889</v>
       </c>
       <c r="G104" t="n">
-        <v>17502.21712230709</v>
+        <v>17502.2171223071</v>
       </c>
       <c r="H104" t="n">
-        <v>39.94413291574746</v>
+        <v>39.94413291574747</v>
       </c>
     </row>
     <row r="105">
@@ -3231,10 +3231,10 @@
         <v>46311.74466304098</v>
       </c>
       <c r="G107" t="n">
-        <v>-7828.618353767932</v>
+        <v>-7828.618353767939</v>
       </c>
       <c r="H107" t="n">
-        <v>-16.90417497921548</v>
+        <v>-16.90417497921549</v>
       </c>
     </row>
     <row r="108">
@@ -3257,10 +3257,10 @@
         <v>38481.76536851194</v>
       </c>
       <c r="G108" t="n">
-        <v>4711.468664511354</v>
+        <v>4711.468664511362</v>
       </c>
       <c r="H108" t="n">
-        <v>12.24337973945072</v>
+        <v>12.24337973945074</v>
       </c>
     </row>
     <row r="109">
@@ -3286,7 +3286,7 @@
         <v>2344.17271103456</v>
       </c>
       <c r="H109" t="n">
-        <v>5.42701613049439</v>
+        <v>5.427016130494391</v>
       </c>
     </row>
     <row r="110">
@@ -3491,10 +3491,10 @@
         <v>20494.89762293924</v>
       </c>
       <c r="G117" t="n">
-        <v>-3326.332074452795</v>
+        <v>-3326.332074452799</v>
       </c>
       <c r="H117" t="n">
-        <v>-16.23004972091076</v>
+        <v>-16.23004972091077</v>
       </c>
     </row>
     <row r="118">
@@ -3595,10 +3595,10 @@
         <v>23150.92995817847</v>
       </c>
       <c r="G121" t="n">
-        <v>5327.554647501969</v>
+        <v>5327.554647501973</v>
       </c>
       <c r="H121" t="n">
-        <v>23.01227059615339</v>
+        <v>23.0122705961534</v>
       </c>
     </row>
     <row r="122">
@@ -3621,10 +3621,10 @@
         <v>28473.33180119714</v>
       </c>
       <c r="G122" t="n">
-        <v>795.4752419654142</v>
+        <v>795.4752419654178</v>
       </c>
       <c r="H122" t="n">
-        <v>2.793755390199783</v>
+        <v>2.793755390199796</v>
       </c>
     </row>
     <row r="123">
@@ -3635,22 +3635,22 @@
         <v>27499.30708977033</v>
       </c>
       <c r="C123" t="n">
-        <v>29534.38401970495</v>
+        <v>29534.38401970496</v>
       </c>
       <c r="D123" t="n">
         <v>26334.81821443653</v>
       </c>
       <c r="E123" t="n">
-        <v>27219.65860811094</v>
+        <v>27219.65860811093</v>
       </c>
       <c r="F123" t="n">
         <v>29227.10398190992</v>
       </c>
       <c r="G123" t="n">
-        <v>-2007.445373798982</v>
+        <v>-2007.445373798986</v>
       </c>
       <c r="H123" t="n">
-        <v>-6.868437512801434</v>
+        <v>-6.868437512801447</v>
       </c>
     </row>
     <row r="124">
@@ -3667,16 +3667,16 @@
         <v>25124.67667984082</v>
       </c>
       <c r="E124" t="n">
-        <v>30477.25128224463</v>
+        <v>30477.25128224462</v>
       </c>
       <c r="F124" t="n">
         <v>27218.41237556436</v>
       </c>
       <c r="G124" t="n">
-        <v>3258.83890668027</v>
+        <v>3258.838906680263</v>
       </c>
       <c r="H124" t="n">
-        <v>11.97292061606771</v>
+        <v>11.97292061606768</v>
       </c>
     </row>
     <row r="125">
@@ -3699,10 +3699,10 @@
         <v>30471.8475630488</v>
       </c>
       <c r="G125" t="n">
-        <v>-1241.736684399788</v>
+        <v>-1241.736684399792</v>
       </c>
       <c r="H125" t="n">
-        <v>-4.075029194834777</v>
+        <v>-4.075029194834788</v>
       </c>
     </row>
     <row r="126">
@@ -3725,10 +3725,10 @@
         <v>29230.87240499029</v>
       </c>
       <c r="G126" t="n">
-        <v>-3299.399511632924</v>
+        <v>-3299.399511632921</v>
       </c>
       <c r="H126" t="n">
-        <v>-11.28737954146607</v>
+        <v>-11.28737954146606</v>
       </c>
     </row>
     <row r="127">
@@ -3739,7 +3739,7 @@
         <v>26306.13632572841</v>
       </c>
       <c r="C127" t="n">
-        <v>27211.11781972406</v>
+        <v>27211.11781972405</v>
       </c>
       <c r="D127" t="n">
         <v>25162.65527224756</v>
@@ -3751,10 +3751,10 @@
         <v>25934.02080615863</v>
       </c>
       <c r="G127" t="n">
-        <v>1033.895494905086</v>
+        <v>1033.895494905089</v>
       </c>
       <c r="H127" t="n">
-        <v>3.986637870898767</v>
+        <v>3.986637870898782</v>
       </c>
     </row>
     <row r="128">
@@ -3781,6 +3781,32 @@
       </c>
       <c r="H128" t="n">
         <v>28.55441258833446</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="n">
+        <v>45260</v>
+      </c>
+      <c r="B129" t="n">
+        <v>35538.26745093573</v>
+      </c>
+      <c r="C129" t="n">
+        <v>37313.96968745709</v>
+      </c>
+      <c r="D129" t="n">
+        <v>34732.3255842841</v>
+      </c>
+      <c r="E129" t="n">
+        <v>37313.96968745709</v>
+      </c>
+      <c r="F129" t="n">
+        <v>34657.27532449595</v>
+      </c>
+      <c r="G129" t="n">
+        <v>2656.694362961134</v>
+      </c>
+      <c r="H129" t="n">
+        <v>7.665618078993555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>